<commit_message>
Published state of ETDataset on 9 August 2018
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy_flexibility_pumped_storage_electricity.converter.xlsx
+++ b/nodes_source_analyses/energy/energy_flexibility_pumped_storage_electricity.converter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorisberkhout/Projects/etdataset/nodes_source_analyses/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B815FA-A019-A441-8843-06D750948CE6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F465D5A-BE9D-5341-BEA2-F18956118418}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27960" windowHeight="16100" tabRatio="762" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27960" windowHeight="16100" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -374,12 +374,19 @@
     <numFmt numFmtId="167" formatCode="0.00000"/>
     <numFmt numFmtId="168" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -868,589 +875,589 @@
   </borders>
   <cellStyleXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="274">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2179,7 +2186,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2214,7 +2221,7 @@
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="161" t="s">
+      <c r="C4" s="152" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2383,8 +2390,8 @@
   </sheetPr>
   <dimension ref="B1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" customHeight="1"/>
@@ -2409,28 +2416,28 @@
       <c r="G1" s="83"/>
     </row>
     <row r="2" spans="2:11" ht="16" customHeight="1">
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="152"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="155"/>
       <c r="F2" s="83"/>
       <c r="G2" s="83"/>
     </row>
     <row r="3" spans="2:11" ht="16" customHeight="1">
-      <c r="B3" s="153"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
-      <c r="E3" s="155"/>
+      <c r="B3" s="156"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="158"/>
       <c r="F3" s="83"/>
       <c r="G3" s="83"/>
     </row>
     <row r="4" spans="2:11" ht="32" customHeight="1">
-      <c r="B4" s="156"/>
-      <c r="C4" s="157"/>
-      <c r="D4" s="157"/>
-      <c r="E4" s="158"/>
+      <c r="B4" s="159"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="161"/>
       <c r="F4" s="83"/>
       <c r="G4" s="83"/>
     </row>
@@ -2506,7 +2513,7 @@
       </c>
       <c r="F10" s="107"/>
       <c r="G10" s="108"/>
-      <c r="I10" s="159" t="s">
+      <c r="I10" s="150" t="s">
         <v>91</v>
       </c>
       <c r="J10" s="95"/>
@@ -2524,7 +2531,7 @@
       </c>
       <c r="F11" s="107"/>
       <c r="G11" s="108"/>
-      <c r="I11" s="159" t="s">
+      <c r="I11" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J11" s="95"/>
@@ -2542,7 +2549,7 @@
       </c>
       <c r="F12" s="107"/>
       <c r="G12" s="108"/>
-      <c r="I12" s="159" t="s">
+      <c r="I12" s="150" t="s">
         <v>91</v>
       </c>
       <c r="J12" s="95"/>
@@ -2556,11 +2563,11 @@
         <v>44</v>
       </c>
       <c r="E13" s="142">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="F13" s="107"/>
       <c r="G13" s="108"/>
-      <c r="I13" s="159" t="s">
+      <c r="I13" s="150" t="s">
         <v>91</v>
       </c>
       <c r="J13" s="95"/>
@@ -2578,7 +2585,7 @@
       </c>
       <c r="F14" s="107"/>
       <c r="G14" s="107"/>
-      <c r="I14" s="159" t="s">
+      <c r="I14" s="150" t="s">
         <v>91</v>
       </c>
       <c r="J14" s="97"/>
@@ -2597,7 +2604,7 @@
       </c>
       <c r="F15" s="107"/>
       <c r="G15" s="107"/>
-      <c r="I15" s="159" t="s">
+      <c r="I15" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J15" s="97"/>
@@ -2616,7 +2623,7 @@
       </c>
       <c r="F16" s="107"/>
       <c r="G16" s="107"/>
-      <c r="I16" s="159" t="s">
+      <c r="I16" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J16" s="97"/>
@@ -2635,7 +2642,7 @@
       </c>
       <c r="F17" s="107"/>
       <c r="G17" s="107"/>
-      <c r="I17" s="159" t="s">
+      <c r="I17" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J17" s="97"/>
@@ -2654,7 +2661,7 @@
       </c>
       <c r="F18" s="107"/>
       <c r="G18" s="107"/>
-      <c r="I18" s="159" t="s">
+      <c r="I18" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J18" s="97"/>
@@ -2673,7 +2680,7 @@
       </c>
       <c r="F19" s="107"/>
       <c r="G19" s="107"/>
-      <c r="I19" s="159" t="s">
+      <c r="I19" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J19" s="97"/>
@@ -2692,7 +2699,7 @@
       </c>
       <c r="F20" s="107"/>
       <c r="G20" s="107"/>
-      <c r="I20" s="159" t="s">
+      <c r="I20" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J20" s="97"/>
@@ -2728,11 +2735,11 @@
         <v>22</v>
       </c>
       <c r="E23" s="110">
-        <v>500000</v>
+        <v>500000000</v>
       </c>
       <c r="F23" s="107"/>
       <c r="G23" s="107"/>
-      <c r="I23" s="159" t="s">
+      <c r="I23" s="150" t="s">
         <v>91</v>
       </c>
       <c r="J23" s="97"/>
@@ -2750,7 +2757,7 @@
       </c>
       <c r="F24" s="107"/>
       <c r="G24" s="107"/>
-      <c r="I24" s="159" t="s">
+      <c r="I24" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J24" s="97"/>
@@ -2768,7 +2775,7 @@
       </c>
       <c r="F25" s="107"/>
       <c r="G25" s="107"/>
-      <c r="I25" s="159" t="s">
+      <c r="I25" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J25" s="97"/>
@@ -2786,7 +2793,7 @@
       </c>
       <c r="F26" s="107"/>
       <c r="G26" s="107"/>
-      <c r="I26" s="159" t="s">
+      <c r="I26" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J26" s="97"/>
@@ -2804,7 +2811,7 @@
       </c>
       <c r="F27" s="107"/>
       <c r="G27" s="107"/>
-      <c r="I27" s="159" t="s">
+      <c r="I27" s="150" t="s">
         <v>91</v>
       </c>
       <c r="J27" s="97"/>
@@ -2822,7 +2829,7 @@
       </c>
       <c r="F28" s="107"/>
       <c r="G28" s="107"/>
-      <c r="I28" s="159" t="s">
+      <c r="I28" s="150" t="s">
         <v>91</v>
       </c>
       <c r="J28" s="97"/>
@@ -2840,7 +2847,7 @@
       </c>
       <c r="F29" s="107"/>
       <c r="G29" s="107"/>
-      <c r="I29" s="159" t="s">
+      <c r="I29" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J29" s="97"/>
@@ -2858,7 +2865,7 @@
       </c>
       <c r="F30" s="107"/>
       <c r="G30" s="107"/>
-      <c r="I30" s="159" t="s">
+      <c r="I30" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J30" s="97"/>
@@ -2876,7 +2883,7 @@
       </c>
       <c r="F31" s="107"/>
       <c r="G31" s="107"/>
-      <c r="I31" s="159" t="s">
+      <c r="I31" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J31" s="97"/>
@@ -2916,7 +2923,7 @@
       </c>
       <c r="F34" s="107"/>
       <c r="G34" s="107"/>
-      <c r="I34" s="159" t="s">
+      <c r="I34" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J34" s="97"/>
@@ -2934,7 +2941,7 @@
       </c>
       <c r="F35" s="107"/>
       <c r="G35" s="107"/>
-      <c r="I35" s="159" t="s">
+      <c r="I35" s="150" t="s">
         <v>91</v>
       </c>
       <c r="J35" s="97"/>
@@ -2952,7 +2959,7 @@
       </c>
       <c r="F36" s="107"/>
       <c r="G36" s="107"/>
-      <c r="I36" s="159" t="s">
+      <c r="I36" s="150" t="s">
         <v>91</v>
       </c>
       <c r="J36" s="97"/>
@@ -2970,7 +2977,7 @@
       </c>
       <c r="F37" s="107"/>
       <c r="G37" s="107"/>
-      <c r="I37" s="159" t="s">
+      <c r="I37" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J37" s="97"/>
@@ -2986,7 +2993,7 @@
       </c>
       <c r="F38" s="107"/>
       <c r="G38" s="107"/>
-      <c r="I38" s="159" t="s">
+      <c r="I38" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J38" s="97"/>
@@ -3002,7 +3009,7 @@
       </c>
       <c r="F39" s="107"/>
       <c r="G39" s="107"/>
-      <c r="I39" s="159" t="s">
+      <c r="I39" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J39" s="97"/>
@@ -3018,7 +3025,7 @@
       </c>
       <c r="F40" s="107"/>
       <c r="G40" s="107"/>
-      <c r="I40" s="159" t="s">
+      <c r="I40" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J40" s="97"/>
@@ -3034,7 +3041,7 @@
       </c>
       <c r="F41" s="107"/>
       <c r="G41" s="107"/>
-      <c r="I41" s="159" t="s">
+      <c r="I41" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J41" s="97"/>
@@ -3050,7 +3057,7 @@
       </c>
       <c r="F42" s="107"/>
       <c r="G42" s="107"/>
-      <c r="I42" s="159" t="s">
+      <c r="I42" s="150" t="s">
         <v>87</v>
       </c>
       <c r="J42" s="97"/>
@@ -3406,13 +3413,13 @@
       </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="C7" s="160" t="s">
+      <c r="C7" s="151" t="s">
         <v>95</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="160" t="s">
+      <c r="F7" s="151" t="s">
         <v>93</v>
       </c>
       <c r="H7" s="133">
@@ -3426,13 +3433,13 @@
       </c>
     </row>
     <row r="8" spans="2:11">
-      <c r="C8" s="160" t="s">
+      <c r="C8" s="151" t="s">
         <v>97</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="160" t="s">
+      <c r="F8" s="151" t="s">
         <v>93</v>
       </c>
       <c r="H8" s="22">

</xml_diff>